<commit_message>
Expanding on gun range concept
</commit_message>
<xml_diff>
--- a/Global Planning Sheet_V08-2021.xlsx
+++ b/Global Planning Sheet_V08-2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\GitHub\Repositories\Minor-Skilled\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75AF0B0C-7207-4F0C-A953-3321FF74BEA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A85F5BC-B1FF-4DD7-8B70-23E9CBAB17D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="887" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="77">
   <si>
     <t xml:space="preserve">Week </t>
   </si>
@@ -287,6 +287,21 @@
   </si>
   <si>
     <t>Research the technologies/algorithms I need to learn about to make the mentioned ideas in the brainstorm document</t>
+  </si>
+  <si>
+    <t>Research existing implementations of mentioned concepts &amp; features</t>
+  </si>
+  <si>
+    <t>Steam pages, promotional content, gameplay videos</t>
+  </si>
+  <si>
+    <t>A document with the technologies/algorithms I have found</t>
+  </si>
+  <si>
+    <t>A document (moodboard?) of the games/implementations I have found</t>
+  </si>
+  <si>
+    <t>A brain</t>
   </si>
 </sst>
 </file>
@@ -938,8 +953,8 @@
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>533361</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>76747</xdr:rowOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>457747</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -954,7 +969,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="260803" y="4943929"/>
+          <a:off x="260803" y="5134429"/>
           <a:ext cx="361004" cy="357961"/>
           <a:chOff x="-47529700" y="2342000"/>
           <a:chExt cx="302450" cy="299900"/>
@@ -1776,7 +1791,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="251898" y="6449785"/>
+          <a:off x="251898" y="7211785"/>
           <a:ext cx="359153" cy="357424"/>
           <a:chOff x="-49786250" y="2316650"/>
           <a:chExt cx="300900" cy="299450"/>
@@ -4233,7 +4248,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="288175" y="8127988"/>
+          <a:off x="288175" y="8889988"/>
           <a:ext cx="358198" cy="272647"/>
           <a:chOff x="-47527350" y="2747625"/>
           <a:chExt cx="300100" cy="228425"/>
@@ -6240,7 +6255,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="288017" y="9670143"/>
+          <a:off x="288017" y="10432143"/>
           <a:ext cx="314006" cy="358229"/>
           <a:chOff x="-46753100" y="1965500"/>
           <a:chExt cx="263075" cy="300125"/>
@@ -13619,7 +13634,7 @@
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13714,7 +13729,9 @@
       <c r="C7" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="27"/>
+      <c r="D7" s="27" t="s">
+        <v>76</v>
+      </c>
       <c r="E7" s="28" t="s">
         <v>69</v>
       </c>
@@ -13731,18 +13748,28 @@
       <c r="D8" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="32"/>
+      <c r="E8" s="32" t="s">
+        <v>74</v>
+      </c>
       <c r="F8" s="33">
         <v>1</v>
       </c>
       <c r="G8" s="34"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B9" s="47"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="33"/>
+      <c r="C9" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="E9" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" s="33">
+        <v>1</v>
+      </c>
       <c r="G9" s="34"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Expanding tank sim concept
</commit_message>
<xml_diff>
--- a/Global Planning Sheet_V08-2021.xlsx
+++ b/Global Planning Sheet_V08-2021.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\GitHub\Repositories\Minor-Skilled\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A85F5BC-B1FF-4DD7-8B70-23E9CBAB17D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B691696-44E6-4108-9487-12C5D41AEFDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="887" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-195" windowWidth="29040" windowHeight="15720" tabRatio="887" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global Planning Sheet" sheetId="7" r:id="rId1"/>
     <sheet name="Global Planning Sheet Example" sheetId="14" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Global Planning Sheet'!$A$1:$H$50</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Global Planning Sheet'!$A$1:$H$49</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Global Planning Sheet Example'!$A$1:$H$50</definedName>
     <definedName name="Stages">#REF!</definedName>
   </definedNames>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="79">
   <si>
     <t xml:space="preserve">Week </t>
   </si>
@@ -301,7 +301,13 @@
     <t>A document (moodboard?) of the games/implementations I have found</t>
   </si>
   <si>
-    <t>A brain</t>
+    <t>A rough idea about the final product.</t>
+  </si>
+  <si>
+    <t>Planning sheet containing the features the MVP should have, with an estimated hour count</t>
+  </si>
+  <si>
+    <t>Plan MVP functionalities, in terms of hours, basic functionality, ranked on importance for the MVP.</t>
   </si>
 </sst>
 </file>
@@ -901,16 +907,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>91257</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>77095</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>136161</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>2257</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1827420</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>20600</xdr:rowOff>
+      <xdr:colOff>1694090</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>757552</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -933,8 +939,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="91257" y="77095"/>
-          <a:ext cx="2100555" cy="881351"/>
+          <a:off x="224607" y="90703"/>
+          <a:ext cx="1557929" cy="755295"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -947,13 +953,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>172357</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>99786</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>533361</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>457747</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -969,7 +975,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="260803" y="5134429"/>
+          <a:off x="260803" y="4467679"/>
           <a:ext cx="361004" cy="357961"/>
           <a:chOff x="-47529700" y="2342000"/>
           <a:chExt cx="302450" cy="299900"/>
@@ -1769,13 +1775,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>163452</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>81642</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>522605</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>58066</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -1791,7 +1797,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="251898" y="7211785"/>
+          <a:off x="251898" y="7116535"/>
           <a:ext cx="359153" cy="357424"/>
           <a:chOff x="-49786250" y="2316650"/>
           <a:chExt cx="300900" cy="299450"/>
@@ -4226,13 +4232,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>199729</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>45345</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>557927</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>127492</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -4248,7 +4254,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="288175" y="8889988"/>
+          <a:off x="288175" y="8794738"/>
           <a:ext cx="358198" cy="272647"/>
           <a:chOff x="-47527350" y="2747625"/>
           <a:chExt cx="300100" cy="228425"/>
@@ -6233,13 +6239,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>199571</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>513577</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>40729</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -6255,7 +6261,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="288017" y="10432143"/>
+          <a:off x="288017" y="10336893"/>
           <a:ext cx="314006" cy="358229"/>
           <a:chOff x="-46753100" y="1965500"/>
           <a:chExt cx="263075" cy="300125"/>
@@ -13628,30 +13634,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:H58"/>
+  <dimension ref="B1:H57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.28515625" style="2" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="40.140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="31.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" style="3" customWidth="1"/>
     <col min="5" max="5" width="27.140625" style="3" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" style="3" customWidth="1"/>
     <col min="7" max="7" width="14.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="21" style="2" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" style="2" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:8" ht="68.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
       <c r="C2" s="45" t="s">
         <v>67</v>
@@ -13678,105 +13684,103 @@
         <v>44970</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="11"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-    </row>
-    <row r="5" spans="2:8" s="4" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="15" t="s">
+    <row r="4" spans="2:8" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D4" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E4" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="17"/>
-      <c r="H5" s="9" t="s">
+      <c r="G4" s="17"/>
+      <c r="H4" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="2:8" s="4" customFormat="1" ht="62.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="18" t="s">
+    <row r="5" spans="2:8" s="4" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="20" t="s">
+      <c r="C5" s="16"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="G6" s="19"/>
-      <c r="H6" s="10" t="s">
+      <c r="G5" s="19"/>
+      <c r="H5" s="10" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="B7" s="46" t="s">
+    <row r="6" spans="2:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="B6" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C6" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="E7" s="28" t="s">
+      <c r="D6" s="27"/>
+      <c r="E6" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="F7" s="29">
+      <c r="F6" s="29">
         <v>1</v>
       </c>
-      <c r="G7" s="30"/>
+      <c r="G6" s="30"/>
+    </row>
+    <row r="7" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B7" s="47"/>
+      <c r="C7" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="F7" s="33">
+        <v>1</v>
+      </c>
+      <c r="G7" s="34"/>
     </row>
     <row r="8" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B8" s="47"/>
       <c r="C8" s="31" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
-      <c r="E8" s="32" t="s">
-        <v>74</v>
+      <c r="E8" s="31" t="s">
+        <v>75</v>
       </c>
       <c r="F8" s="33">
         <v>1</v>
       </c>
       <c r="G8" s="34"/>
     </row>
-    <row r="9" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="47"/>
-      <c r="C9" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="D9" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="E9" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="F9" s="33">
-        <v>1</v>
-      </c>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="33"/>
       <c r="G9" s="34"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="47"/>
       <c r="C10" s="31"/>
       <c r="D10" s="31"/>
-      <c r="E10" s="32"/>
+      <c r="E10" s="31"/>
       <c r="F10" s="33"/>
       <c r="G10" s="34"/>
     </row>
@@ -13789,7 +13793,7 @@
       <c r="G11" s="34"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="47"/>
+      <c r="B12" s="48"/>
       <c r="C12" s="31"/>
       <c r="D12" s="31"/>
       <c r="E12" s="31"/>
@@ -13797,25 +13801,31 @@
       <c r="G12" s="34"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="48"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="34"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="25"/>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="22"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="25"/>
+    <row r="14" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B14" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="F14" s="36"/>
+      <c r="G14" s="37"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="49" t="s">
-        <v>53</v>
-      </c>
+      <c r="B15" s="50"/>
       <c r="C15" s="35"/>
       <c r="D15" s="35"/>
       <c r="E15" s="35"/>
@@ -13848,14 +13858,14 @@
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="50"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
       <c r="E19" s="35"/>
       <c r="F19" s="36"/>
       <c r="G19" s="37"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="50"/>
+      <c r="B20" s="51"/>
       <c r="C20" s="38"/>
       <c r="D20" s="38"/>
       <c r="E20" s="35"/>
@@ -13863,25 +13873,25 @@
       <c r="G20" s="37"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="51"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="37"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="25"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="26"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="25"/>
+      <c r="B22" s="49" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="41"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="49" t="s">
-        <v>54</v>
-      </c>
+      <c r="B23" s="50"/>
       <c r="C23" s="39"/>
       <c r="D23" s="39"/>
       <c r="E23" s="39"/>
@@ -13929,7 +13939,7 @@
       <c r="G28" s="41"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="50"/>
+      <c r="B29" s="51"/>
       <c r="C29" s="39"/>
       <c r="D29" s="39"/>
       <c r="E29" s="39"/>
@@ -13937,25 +13947,25 @@
       <c r="G29" s="41"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="51"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="41"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="25"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="26"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="25"/>
+      <c r="B31" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="43"/>
+      <c r="G31" s="44"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="49" t="s">
-        <v>55</v>
-      </c>
+      <c r="B32" s="50"/>
       <c r="C32" s="42"/>
       <c r="D32" s="42"/>
       <c r="E32" s="42"/>
@@ -13995,7 +14005,7 @@
       <c r="G36" s="44"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="50"/>
+      <c r="B37" s="51"/>
       <c r="C37" s="42"/>
       <c r="D37" s="42"/>
       <c r="E37" s="42"/>
@@ -14003,29 +14013,25 @@
       <c r="G37" s="44"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="51"/>
-      <c r="C38" s="42"/>
-      <c r="D38" s="42"/>
-      <c r="E38" s="42"/>
-      <c r="F38" s="43"/>
-      <c r="G38" s="44"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="25"/>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="26"/>
-      <c r="C39" s="23"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="23"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="25"/>
+      <c r="B39" s="2"/>
+      <c r="G39" s="3"/>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="2"/>
+    <row r="40" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B40" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="G40" s="3"/>
     </row>
-    <row r="41" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B41" s="3" t="s">
-        <v>45</v>
-      </c>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="3"/>
       <c r="G41" s="3"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
@@ -14056,11 +14062,11 @@
       <c r="B48" s="3"/>
       <c r="G48" s="3"/>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="3"/>
       <c r="G49" s="3"/>
     </row>
-    <row r="50" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="3"/>
       <c r="G50" s="3"/>
     </row>
@@ -14092,16 +14098,12 @@
       <c r="B57" s="3"/>
       <c r="G57" s="3"/>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B58" s="3"/>
-      <c r="G58" s="3"/>
-    </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="B7:B13"/>
-    <mergeCell ref="B15:B21"/>
-    <mergeCell ref="B23:B30"/>
-    <mergeCell ref="B32:B38"/>
+    <mergeCell ref="B6:B12"/>
+    <mergeCell ref="B14:B20"/>
+    <mergeCell ref="B22:B29"/>
+    <mergeCell ref="B31:B37"/>
     <mergeCell ref="D2:G2"/>
     <mergeCell ref="E3:F3"/>
   </mergeCells>
@@ -14116,7 +14118,7 @@
   <dimension ref="B1:H58"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
       <selection pane="bottomRight" activeCell="D36" sqref="D36"/>

</xml_diff>

<commit_message>
Worked on gun range concept (finalized?)
</commit_message>
<xml_diff>
--- a/Global Planning Sheet_V08-2021.xlsx
+++ b/Global Planning Sheet_V08-2021.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\GitHub\Repositories\Minor-Skilled\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\GitHub\Repositories\Minor-Skilled-Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B691696-44E6-4108-9487-12C5D41AEFDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07146949-16F4-4DC5-8391-8BE2AE927ABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-195" windowWidth="29040" windowHeight="15720" tabRatio="887" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="83">
   <si>
     <t xml:space="preserve">Week </t>
   </si>
@@ -307,7 +307,19 @@
     <t>Planning sheet containing the features the MVP should have, with an estimated hour count</t>
   </si>
   <si>
-    <t>Plan MVP functionalities, in terms of hours, basic functionality, ranked on importance for the MVP.</t>
+    <t>Plan/design MVP mechanics</t>
+  </si>
+  <si>
+    <t>Make planning/estimated hour registration for mechanics. Rank importance for MVP. Highest priority first</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An estimation of time for each feature. </t>
+  </si>
+  <si>
+    <t>A design document describing the mechanics for the concept I have chosen</t>
+  </si>
+  <si>
+    <t>Inspiritation from several sources (existing games, prototype demos on youtube), an estimation of what I can do in 5 months</t>
   </si>
 </sst>
 </file>
@@ -1797,7 +1809,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="251898" y="7116535"/>
+          <a:off x="251898" y="7497535"/>
           <a:ext cx="359153" cy="357424"/>
           <a:chOff x="-49786250" y="2316650"/>
           <a:chExt cx="300900" cy="299450"/>
@@ -4254,7 +4266,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="288175" y="8794738"/>
+          <a:off x="288175" y="9175738"/>
           <a:ext cx="358198" cy="272647"/>
           <a:chOff x="-47527350" y="2747625"/>
           <a:chExt cx="300100" cy="228425"/>
@@ -6261,7 +6273,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="288017" y="10336893"/>
+          <a:off x="288017" y="10717893"/>
           <a:ext cx="314006" cy="358229"/>
           <a:chOff x="-46753100" y="1965500"/>
           <a:chExt cx="263075" cy="300125"/>
@@ -13637,10 +13649,10 @@
   <dimension ref="B1:H57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13681,7 +13693,7 @@
       <c r="F3" s="55"/>
       <c r="G3" s="8">
         <f ca="1">(TODAY())</f>
-        <v>44970</v>
+        <v>44971</v>
       </c>
     </row>
     <row r="4" spans="2:8" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -13727,7 +13739,9 @@
       <c r="C6" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="D6" s="27"/>
+      <c r="D6" s="27" t="s">
+        <v>82</v>
+      </c>
       <c r="E6" s="28" t="s">
         <v>69</v>
       </c>
@@ -13808,7 +13822,7 @@
       <c r="F13" s="24"/>
       <c r="G13" s="25"/>
     </row>
-    <row r="14" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B14" s="49" t="s">
         <v>53</v>
       </c>
@@ -13819,17 +13833,27 @@
         <v>76</v>
       </c>
       <c r="E14" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" s="36">
+        <v>1</v>
+      </c>
+      <c r="G14" s="37"/>
+    </row>
+    <row r="15" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B15" s="50"/>
+      <c r="C15" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="F14" s="36"/>
-      <c r="G14" s="37"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="50"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="36"/>
+      <c r="F15" s="36">
+        <v>1</v>
+      </c>
       <c r="G15" s="37"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
@@ -14162,7 +14186,7 @@
       <c r="F3" s="55"/>
       <c r="G3" s="8">
         <f ca="1">(TODAY())</f>
-        <v>44970</v>
+        <v>44971</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>